<commit_message>
So I made some changes
</commit_message>
<xml_diff>
--- a/funvalues.xlsx
+++ b/funvalues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Stuff\Games\Games\The Binding of Isaac Rebirth Repentance\mods\Dies Irae\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C137EE-4BCC-4CA1-8881-839A16BAF800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8BDC615-2CBA-46A9-82BB-4684A11BA090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5B11D2BD-403F-41C2-9727-449EEB2CE6F3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="116">
   <si>
     <t>FUN Value!!</t>
   </si>
@@ -373,6 +373,15 @@
   </si>
   <si>
     <t>You know it won't change</t>
+  </si>
+  <si>
+    <t>Monster Isaac</t>
+  </si>
+  <si>
+    <t>Upon death, Isaac transform into Gaper</t>
+  </si>
+  <si>
+    <t>Short in-game cutscene</t>
   </si>
 </sst>
 </file>
@@ -817,8 +826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65207D12-6352-407B-9464-4AD8EE01CF17}">
   <dimension ref="A1:W22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1533,30 +1542,38 @@
       <c r="V16" s="3"/>
       <c r="W16" s="3"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
-      <c r="U17" s="5"/>
-      <c r="V17" s="5"/>
-      <c r="W17" s="5"/>
+    <row r="17" spans="1:23" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
+      <c r="U17" s="3"/>
+      <c r="V17" s="3"/>
+      <c r="W17" s="3"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>

</xml_diff>